<commit_message>
Còn thiếu import bằng file, UNC ĐATN ( chờ P ) và chỉnh lại save các file
</commit_message>
<xml_diff>
--- a/src/templates/uy-nhiem-chi/Mẫu Ủy Nhiệm Chi Mật Mã.xlsx
+++ b/src/templates/uy-nhiem-chi/Mẫu Ủy Nhiệm Chi Mật Mã.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94ED1A29-0932-461D-9BCC-3C43A3C0A6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41B3E35-FB87-4AE4-9FD7-AA230DBC4C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,12 +40,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>ỦY NHIỆM CHI</t>
-  </si>
-  <si>
-    <t>STT</t>
   </si>
   <si>
     <r>
@@ -217,59 +214,6 @@
     <t>Tại kho bạc Nhà nước (NH):</t>
   </si>
   <si>
-    <r>
-      <t>Số CMND:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> ………………...……</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Cấp ngày:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> …...……………………</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Nơi cấp: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>…………………</t>
-    </r>
-  </si>
-  <si>
     <t>KHO BẠC NHÀ NƯỚC</t>
   </si>
   <si>
@@ -300,9 +244,6 @@
     <t>{{nien_do}}</t>
   </si>
   <si>
-    <t>{{so _tien}}</t>
-  </si>
-  <si>
     <t>{{tai_khoan_thanh_toan}}</t>
   </si>
   <si>
@@ -310,6 +251,24 @@
   </si>
   <si>
     <t>{{don_vi_nhan}}</t>
+  </si>
+  <si>
+    <t>{{tai_khoan}}</t>
+  </si>
+  <si>
+    <t>{{kho_bac}}</t>
+  </si>
+  <si>
+    <t>Ngày       tháng     năm 2025</t>
+  </si>
+  <si>
+    <t>{{noi_dung_thanh_toan}}</t>
+  </si>
+  <si>
+    <t>Người nhận tiền: {{nguoi_nhan_tien}}</t>
+  </si>
+  <si>
+    <t>Số CMND: {{CCCD}} Cấp ngày: {{ngay_cap}} Nơi cấp: {{noi_cap}}</t>
   </si>
   <si>
     <r>
@@ -325,31 +284,12 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="163"/>
-      </rPr>
-      <t>{{dia_chi}}</t>
-    </r>
   </si>
   <si>
-    <t>{{tai_khoan}}</t>
+    <t>{{dia_chi}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Người nhận tiền: </t>
-  </si>
-  <si>
-    <t>{{kho_bac}}</t>
-  </si>
-  <si>
-    <t>Ngày       tháng     năm 2025</t>
-  </si>
-  <si>
-    <t>{{noi_dung_thanh_toan}}</t>
+    <t>{{so_tien}}</t>
   </si>
 </sst>
 </file>
@@ -626,15 +566,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -671,16 +605,37 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -704,41 +659,26 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -860,15 +800,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>97155</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:colOff>1325880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>155575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -885,8 +825,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5276850" y="57150"/>
-          <a:ext cx="1228725" cy="762000"/>
+          <a:off x="5481955" y="107950"/>
+          <a:ext cx="1228725" cy="748665"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5052,10 +4992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -5450,63 +5390,57 @@
     <col min="16138" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="1">
-        <v>888</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="46" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="46" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+    </row>
+    <row r="5" spans="1:9" ht="23.25" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-    </row>
-    <row r="5" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -5515,12 +5449,12 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="23.25" customHeight="1">
+    <row r="6" spans="1:9" ht="23.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -5530,9 +5464,9 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="23.25" customHeight="1">
+    <row r="7" spans="1:9" ht="23.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -5542,12 +5476,12 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:10" s="5" customFormat="1" ht="23.25" customHeight="1">
+    <row r="8" spans="1:9" s="5" customFormat="1" ht="23.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -5556,9 +5490,9 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:10" s="5" customFormat="1" ht="23.25" customHeight="1">
+    <row r="9" spans="1:9" s="5" customFormat="1" ht="23.25" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -5568,275 +5502,276 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:10" s="8" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A10" s="48" t="s">
+    <row r="10" spans="1:9" s="8" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A10" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="7" t="s">
+    </row>
+    <row r="11" spans="1:9" s="11" customFormat="1" ht="16.8">
+      <c r="A11" s="30" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" s="11" customFormat="1" ht="16.8">
-      <c r="A11" s="51" t="s">
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="H11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="10" t="s">
+    </row>
+    <row r="12" spans="1:9" s="11" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A12" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" s="5" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A13" s="43" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" s="11" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A12" s="35" t="s">
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="12" t="s">
-        <v>31</v>
+    </row>
+    <row r="14" spans="1:9" s="16" customFormat="1" ht="42.6" customHeight="1">
+      <c r="A14" s="46" t="s">
+        <v>17</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>32</v>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="49" t="s">
+        <v>28</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1">
+      <c r="A15" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="47"/>
+      <c r="C15" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="15"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
     </row>
-    <row r="13" spans="1:10" s="5" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A13" s="38" t="s">
-        <v>17</v>
+    <row r="16" spans="1:9" ht="23.25" customHeight="1">
+      <c r="A16" s="18" t="s">
+        <v>40</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="16" t="str">
-        <f>H12</f>
-        <v>{{so _tien}}</v>
+      <c r="B16" s="39" t="s">
+        <v>41</v>
       </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
     </row>
-    <row r="14" spans="1:10" s="18" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A14" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="42"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-    </row>
-    <row r="15" spans="1:10" ht="30" customHeight="1">
-      <c r="A15" s="43" t="s">
+    <row r="17" spans="1:8" ht="27" customHeight="1">
+      <c r="A17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-    </row>
-    <row r="16" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A16" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-    </row>
-    <row r="17" spans="1:8" ht="27" customHeight="1">
-      <c r="A17" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>38</v>
+      <c r="B17" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+    </row>
+    <row r="19" spans="1:8" ht="27" customHeight="1">
+      <c r="A19" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+    </row>
+    <row r="20" spans="1:8" ht="30" customHeight="1">
+      <c r="A20" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+    </row>
+    <row r="21" spans="1:8" ht="9" customHeight="1">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+    </row>
+    <row r="22" spans="1:8" s="21" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A22" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-    </row>
-    <row r="19" spans="1:8" ht="27" customHeight="1">
-      <c r="A19" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-    </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1">
-      <c r="A20" s="33" t="s">
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
+      <c r="H22" s="50"/>
     </row>
-    <row r="21" spans="1:8" ht="9" customHeight="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="22" spans="1:8" s="23" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A22" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" s="31"/>
-    </row>
-    <row r="23" spans="1:8" s="25" customFormat="1" ht="36" customHeight="1">
-      <c r="A23" s="31" t="str">
+    <row r="23" spans="1:8" s="23" customFormat="1" ht="36" customHeight="1">
+      <c r="A23" s="50" t="str">
         <f>G23</f>
         <v>Ngày       tháng     năm 2025</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="24" t="s">
-        <v>25</v>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="22" t="s">
+        <v>23</v>
       </c>
-      <c r="G23" s="31" t="str">
+      <c r="G23" s="50" t="str">
         <f>A4</f>
         <v>Ngày       tháng     năm 2025</v>
       </c>
-      <c r="H23" s="31"/>
+      <c r="H23" s="50"/>
     </row>
-    <row r="24" spans="1:8" s="26" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A24" s="31" t="s">
+    <row r="24" spans="1:8" s="24" customFormat="1" ht="40.200000000000003" customHeight="1">
+      <c r="A24" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="24" t="s">
+      <c r="H24" s="51"/>
+    </row>
+    <row r="25" spans="1:8" s="24" customFormat="1">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="H24" s="32"/>
+      <c r="H25" s="27"/>
     </row>
-    <row r="25" spans="1:8" s="26" customFormat="1">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="H25" s="29"/>
+    <row r="26" spans="1:8" s="24" customFormat="1">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
     </row>
-    <row r="26" spans="1:8" s="26" customFormat="1">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
+    <row r="27" spans="1:8" s="24" customFormat="1">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
     </row>
-    <row r="27" spans="1:8" s="26" customFormat="1">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+    <row r="28" spans="1:8" s="24" customFormat="1">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
     </row>
-    <row r="28" spans="1:8" s="26" customFormat="1">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-    </row>
-    <row r="29" spans="1:8" s="26" customFormat="1">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="24" t="str">
+    <row r="29" spans="1:8" s="24" customFormat="1">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="22" t="str">
         <f>'[1]3 (25'!E30</f>
         <v>Hoàng Văn Thức</v>
       </c>
@@ -5863,29 +5798,29 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="D14:H14"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="G22:H22"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0" top="0.47244094488188981" bottom="0.47244094488188981" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="97" orientation="portrait" r:id="rId1"/>

</xml_diff>